<commit_message>
added MICROSMD010 to list
</commit_message>
<xml_diff>
--- a/HW_COMPONENTS/BOM/BOM_pocket_sdr_v2.1_NEO.xlsx
+++ b/HW_COMPONENTS/BOM/BOM_pocket_sdr_v2.1_NEO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenchitaru-alex\Documents\EAGLE\projects\PocketSDR\kicad\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenchitaru-alex\Documents\GitHub\PocketSDRNEO\HW_COMPONENTS\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{969BF55C-BE1D-441D-AEAC-0B9DE55A3E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76631F46-D9D0-4629-BD2D-CAA2F98D9716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57840" yWindow="17550" windowWidth="31920" windowHeight="28215"/>
+    <workbookView xWindow="5070" yWindow="4185" windowWidth="31920" windowHeight="28215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pocket_sdr_v2.1_NEO" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="289">
   <si>
     <t>Index</t>
   </si>
@@ -851,13 +851,49 @@
   </si>
   <si>
     <t>https://www.mouser.jp/ProductDetail/Analog-Devices-Maxim-Integrated/MAX2771ETI%2b?qs=lc2O%252BfHJPVYuzqxyqJXfmg%3D%3D</t>
+  </si>
+  <si>
+    <t>MICROSMD010F-2</t>
+  </si>
+  <si>
+    <t>Littelfuse Inc.</t>
+  </si>
+  <si>
+    <t>PTC RESET FUSE 30V 100MA 1210</t>
+  </si>
+  <si>
+    <t>MICROSMD010F-2CT-ND</t>
+  </si>
+  <si>
+    <t>55.00000</t>
+  </si>
+  <si>
+    <t>¥55</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>https://www.littelfuse.com/~/media/electronics/product_specifications/resettable_ptcs/littelfuse_ptc_microsmd010f_2_product_specification.pdf.pdf</t>
+  </si>
+  <si>
+    <t>2A  (4 Weeks)</t>
+  </si>
+  <si>
+    <t>8533.40.8070</t>
+  </si>
+  <si>
+    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/images/3007/MICROSMDF SERIES.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1012,6 +1048,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1348,7 +1388,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1392,24 +1432,27 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="43"/>
+    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="43" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1448,6 +1491,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="43" xr:uid="{22528E0A-7E81-400B-A682-5DD7727D8740}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1763,14 +1807,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AD45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.85546875" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
@@ -1779,14 +1823,14 @@
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:30" ht="45" customHeight="1">
+      <c r="A1" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1878,7 +1922,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1958,7 +2002,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2038,7 +2082,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2115,7 +2159,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2195,7 +2239,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2275,7 +2319,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2355,7 +2399,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2435,7 +2479,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2515,7 +2559,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2595,7 +2639,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2672,7 +2716,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2749,7 +2793,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2826,7 +2870,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2903,7 +2947,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2980,7 +3024,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3057,7 +3101,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3134,7 +3178,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3211,7 +3255,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3288,7 +3332,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3365,7 +3409,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3445,7 +3489,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3522,7 +3566,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3599,7 +3643,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3679,7 +3723,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3759,7 +3803,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3839,7 +3883,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3919,7 +3963,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3996,7 +4040,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30">
       <c r="A30">
         <v>28</v>
       </c>
@@ -4073,7 +4117,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30">
       <c r="A31">
         <v>29</v>
       </c>
@@ -4153,7 +4197,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30">
       <c r="A32">
         <v>30</v>
       </c>
@@ -4233,180 +4277,272 @@
         <v>244</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+    <row r="33" spans="1:30">
+      <c r="A33" s="8">
+        <v>31</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="E33" s="9">
+        <v>82922</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8">
+        <v>1</v>
+      </c>
+      <c r="I33" s="8">
+        <v>1</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="L33" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="M33" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="N33" s="8">
+        <v>1</v>
+      </c>
+      <c r="O33" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="P33" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q33" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="R33" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="S33" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="T33" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="U33" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="V33" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="W33" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="X33" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="Y33" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z33" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="AA33" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB33" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="AC33" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="AD33" s="8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" ht="45" customHeight="1">
+      <c r="A36" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="7"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:30">
+      <c r="A37" t="s">
         <v>247</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>248</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>249</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>3</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>250</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" t="s">
         <v>251</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G37" t="s">
         <v>252</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H37" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="38" spans="1:30">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
         <v>253</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>254</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>255</v>
       </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
         <v>256</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G38" t="s">
         <v>256</v>
       </c>
-      <c r="H37" s="7" t="s">
+      <c r="H38" s="4" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="39" spans="1:30">
+      <c r="A39">
         <v>2</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>257</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>258</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>259</v>
       </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
         <v>260</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G39" t="s">
         <v>260</v>
       </c>
-      <c r="H38" s="7" t="s">
+      <c r="H39" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="40" spans="1:30">
+      <c r="A40">
         <v>3</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>272</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>273</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>274</v>
       </c>
-      <c r="E39">
+      <c r="E40">
         <v>2</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" t="s">
         <v>275</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G40" t="s">
         <v>275</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H40" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+    <row r="43" spans="1:30" ht="45" customHeight="1">
+      <c r="A43" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="5"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="7"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:30">
+      <c r="A44" t="s">
         <v>0</v>
       </c>
-      <c r="B43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
         <v>3</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>250</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E44" t="s">
         <v>270</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F44" t="s">
         <v>268</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G44" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44" t="s">
+    <row r="45" spans="1:30">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
         <v>266</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>267</v>
       </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44">
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
         <v>10</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F45" t="s">
         <v>269</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G45" t="s">
         <v>271</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A43:C43"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H37" r:id="rId1"/>
-    <hyperlink ref="H38" r:id="rId2"/>
+    <hyperlink ref="H38" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H39" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="R33" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="AD33" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>